<commit_message>
Include openpyxl and pandas in requirements.txt
</commit_message>
<xml_diff>
--- a/dimension_sheet.xlsx
+++ b/dimension_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poome\GitHub\CCF_Paybill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4786B68B-A77E-4CC0-8615-C409704BE74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86161A04-B59B-4DDE-9588-4CB17D8C9792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payment_type" sheetId="1" r:id="rId1"/>
@@ -1195,7 +1195,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1283,13 +1283,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{8E1EA9F4-52B3-4B50-96E5-7A66A5F7EED3}"/>
     <cellStyle name="Percent 2" xfId="2" xr:uid="{DAB7729D-FB7E-42E1-9C15-1DCFDDFA7A45}"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="19">
     <dxf>
       <font>
         <b/>
@@ -1305,88 +1312,25 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
+      <alignment horizontal="right"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
+      <alignment horizontal="right"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <name val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1479,6 +1423,24 @@
         <strike val="0"/>
         <u val="none"/>
         <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Tahoma"/>
         <family val="2"/>
@@ -1497,24 +1459,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1593,8 +1537,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4093A9C5-B06F-4966-82C7-3BC1DFDADF78}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0">
   <autoFilter ref="A1:B5" xr:uid="{4093A9C5-B06F-4966-82C7-3BC1DFDADF78}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{002D0D7D-2632-45DA-8897-E03350DBDFAD}" name="รหัส" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{3DD8E6F5-E361-4744-8F9D-8893654180AF}" name="ประเภทการจ่าย" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{002D0D7D-2632-45DA-8897-E03350DBDFAD}" name="รหัส" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{3DD8E6F5-E361-4744-8F9D-8893654180AF}" name="ประเภทการจ่าย" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1604,20 +1548,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC38BFD9-64AD-4BF8-AC28-F6AFBAEEBA37}" name="Table7" displayName="Table7" ref="A1:H13" totalsRowShown="0">
   <autoFilter ref="A1:H13" xr:uid="{CC38BFD9-64AD-4BF8-AC28-F6AFBAEEBA37}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D796B34F-DB88-4876-A39D-AB16EE498D63}" name="รหัส" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{6EC6A6D2-CAC3-4C08-AC8A-1F96A9C232F3}" name="งวดเดือน" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{30ED3D52-DB2A-4C2A-8417-BBF3664C0F20}" name="ประจำงวดวันที่" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{D796B34F-DB88-4876-A39D-AB16EE498D63}" name="รหัส" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{6EC6A6D2-CAC3-4C08-AC8A-1F96A9C232F3}" name="งวดเดือน" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{30ED3D52-DB2A-4C2A-8417-BBF3664C0F20}" name="ประจำงวดวันที่" dataDxfId="14">
       <calculatedColumnFormula>TEXT(Table7[[#This Row],[เริ่มงวด]],"dd/mm")&amp;" - "&amp;TEXT(Table7[[#This Row],[จบงวด]],"dd/mm/yy")&amp;" ("&amp;A2&amp;")"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{83361EEF-5901-4637-8C3A-20CF00002B6F}" name="วันที่จ่ายเงินเดือน" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{EE7AFBD0-20E0-4E3C-9E8F-7DA31056FEE0}" name="เริ่มงวด" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{D2EC60E8-6F2E-411D-B05C-5C35C3830E1B}" name="จบงวด" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{83361EEF-5901-4637-8C3A-20CF00002B6F}" name="วันที่จ่ายเงินเดือน" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{EE7AFBD0-20E0-4E3C-9E8F-7DA31056FEE0}" name="เริ่มงวด" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{D2EC60E8-6F2E-411D-B05C-5C35C3830E1B}" name="จบงวด" dataDxfId="11">
       <calculatedColumnFormula>DATE(YEAR(E2),MONTH(E2)+1,25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3B0A67D-94C5-4351-A5E5-FB9B3CF22851}" name="จำนวนวัน" dataDxfId="14">
+    <tableColumn id="8" xr3:uid="{C3B0A67D-94C5-4351-A5E5-FB9B3CF22851}" name="จำนวนวัน" dataDxfId="10">
       <calculatedColumnFormula>Table7[[#This Row],[จบงวด]]-Table7[[#This Row],[เริ่มงวด]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{26AB2C1F-B148-419E-A936-9886B3EBAE42}" name="กำหนดวันทำงานเบี้ยขยัน" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{26AB2C1F-B148-419E-A936-9886B3EBAE42}" name="กำหนดวันทำงานเบี้ยขยัน" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1641,18 +1585,18 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{9917D4C7-225C-47C0-A1D4-9DE0CB9FEA0F}" name="ลำดับ" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{9917D4C7-225C-47C0-A1D4-9DE0CB9FEA0F}" name="ลำดับ" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{B5648327-2131-49D2-AF74-1D00B508E7D6}" name="รหัสพนักงาน"/>
     <tableColumn id="3" xr3:uid="{87B4C719-52BD-4A74-8C10-D714692DEA82}" name="ชื่อพนักงาน"/>
     <tableColumn id="4" xr3:uid="{75B585FC-C32B-4FE2-B430-FFC4FE5D9487}" name="ชื่อพนักงาน ID"/>
-    <tableColumn id="5" xr3:uid="{29A8B304-D0E7-4F55-8834-0BA7E6CFA908}" name="สังกัดฝ่าย" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{55654F1D-DC7E-43B0-A34C-97A397655842}" name="Department" dataDxfId="11" dataCellStyle="Normal 2"/>
-    <tableColumn id="6" xr3:uid="{23C6A94E-3EF0-4AC5-BC20-6213EBB7557C}" name="ระดับขั้นพนักงาน (Level)" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{F793CA5E-0452-4586-A0C0-3F58670D221F}" name="ฐานค่าแรง" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{9AFD31E3-A194-4CCF-A3A8-F5A33E2DBA16}" name="ช่องทางจ่ายเงินเดือน" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{29A8B304-D0E7-4F55-8834-0BA7E6CFA908}" name="สังกัดฝ่าย" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{55654F1D-DC7E-43B0-A34C-97A397655842}" name="Department" dataDxfId="6" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" xr3:uid="{23C6A94E-3EF0-4AC5-BC20-6213EBB7557C}" name="ระดับขั้นพนักงาน (Level)" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{F793CA5E-0452-4586-A0C0-3F58670D221F}" name="ฐานค่าแรง" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{9AFD31E3-A194-4CCF-A3A8-F5A33E2DBA16}" name="ช่องทางจ่ายเงินเดือน" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{D0199BE2-EE61-4F36-9A66-FDBCB9764868}" name="วิธีการจ่ายเงินเดือน"/>
     <tableColumn id="10" xr3:uid="{9F725C4E-8BC1-4396-B3CD-34E30054C215}" name="ประเภทพนักนักงาน"/>
-    <tableColumn id="11" xr3:uid="{78272A7F-EADA-4C5C-8C53-27625766BF45}" name="ช่องทางการจ่ายเงินเดือน2" dataDxfId="22">
+    <tableColumn id="11" xr3:uid="{78272A7F-EADA-4C5C-8C53-27625766BF45}" name="ช่องทางการจ่ายเงินเดือน2" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(Table4[[#This Row],[ช่องทางจ่ายเงินเดือน]],[1]!Table2[#Data],2,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{70A6F726-7666-40C9-BFB4-7DAAE955984C}" name="% หักปกส."/>
@@ -2002,16 +1946,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0227CBE1-0E70-4BB5-98DF-C8E085F2F3EA}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2021,10 +1965,12 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J2" s="39"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="39"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>0</v>
       </c>
@@ -2032,13 +1978,15 @@
         <v>0</v>
       </c>
       <c r="C3" s="6">
-        <f>B3*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C3:C19" si="0">B3*$K$4</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="39"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="39"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2046,13 +1994,15 @@
         <v>0.01</v>
       </c>
       <c r="C4" s="11">
-        <f>B4*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="13"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="39"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="39"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2060,13 +2010,15 @@
         <v>0.02</v>
       </c>
       <c r="C5" s="11">
-        <f>B5*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="13"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="39"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="39"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2074,13 +2026,15 @@
         <v>0.03</v>
       </c>
       <c r="C6" s="11">
-        <f>B6*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="13"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="39"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="39"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2088,13 +2042,15 @@
         <v>0.04</v>
       </c>
       <c r="C7" s="11">
-        <f>B7*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="13"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="39"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="39"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2102,13 +2058,15 @@
         <v>0.05</v>
       </c>
       <c r="C8" s="11">
-        <f>B8*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="13"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="39"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="39"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2116,13 +2074,15 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="C9" s="11">
-        <f>B9*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="13"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="39"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="39"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2130,13 +2090,15 @@
         <v>0.08</v>
       </c>
       <c r="C10" s="11">
-        <f>B10*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="39"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="39"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2144,13 +2106,15 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="C11" s="11">
-        <f>B11*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="13"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="39"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="39"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2159,13 +2123,15 @@
         <v>0.11</v>
       </c>
       <c r="C12" s="11">
-        <f>B12*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="13"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="39"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="39"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2174,13 +2140,15 @@
         <v>0.125</v>
       </c>
       <c r="C13" s="11">
-        <f>B13*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="39"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="39"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2189,86 +2157,98 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="C14" s="11">
-        <f>B14*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="39"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="39"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
       <c r="B15" s="10">
-        <f t="shared" ref="B15:B19" si="0">B14+0.02</f>
+        <f t="shared" ref="B15:B19" si="1">B14+0.02</f>
         <v>0.16499999999999998</v>
       </c>
       <c r="C15" s="11">
-        <f>B15*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="39"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="39"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>13</v>
       </c>
       <c r="B16" s="10">
+        <f t="shared" si="1"/>
+        <v>0.18499999999999997</v>
+      </c>
+      <c r="C16" s="11">
         <f t="shared" si="0"/>
-        <v>0.18499999999999997</v>
-      </c>
-      <c r="C16" s="11">
-        <f>B16*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J16" s="39"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="39"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>14</v>
       </c>
       <c r="B17" s="10">
+        <f t="shared" si="1"/>
+        <v>0.20499999999999996</v>
+      </c>
+      <c r="C17" s="11">
         <f t="shared" si="0"/>
-        <v>0.20499999999999996</v>
-      </c>
-      <c r="C17" s="11">
-        <f>B17*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="39"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="39"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16">
         <v>15</v>
       </c>
       <c r="B18" s="17">
+        <f t="shared" si="1"/>
+        <v>0.22499999999999995</v>
+      </c>
+      <c r="C18" s="18">
         <f t="shared" si="0"/>
-        <v>0.22499999999999995</v>
-      </c>
-      <c r="C18" s="18">
-        <f>B18*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K18" s="19"/>
-      <c r="L18" s="20"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="39"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="39"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <v>16</v>
       </c>
       <c r="B19" s="17">
+        <f t="shared" si="1"/>
+        <v>0.24499999999999994</v>
+      </c>
+      <c r="C19" s="18">
         <f t="shared" si="0"/>
-        <v>0.24499999999999994</v>
-      </c>
-      <c r="C19" s="18">
-        <f>B19*$K$4</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="19"/>
-      <c r="L19" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="39"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2561,7 +2541,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2964,7 +2944,7 @@
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6379,58 +6359,13 @@
       <c r="M95" s="36"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J50 J64:J95">
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="เงินสด">
-      <formula>NOT(ISERROR(SEARCH("เงินสด",J50)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K50 K65:K95">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="รายเดือน">
-      <formula>NOT(ISERROR(SEARCH("รายเดือน",K50)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K56">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="รายเดือน">
-      <formula>NOT(ISERROR(SEARCH("รายเดือน",K56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J20">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="เงินสด">
-      <formula>NOT(ISERROR(SEARCH("เงินสด",J20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J34:J36">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="เงินสด">
-      <formula>NOT(ISERROR(SEARCH("เงินสด",J34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J51:J55">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="เงินสด">
-      <formula>NOT(ISERROR(SEARCH("เงินสด",J51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19:K20">
-    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="รายเดือน">
-      <formula>NOT(ISERROR(SEARCH("รายเดือน",K19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K34:K36">
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="รายเดือน">
-      <formula>NOT(ISERROR(SEARCH("รายเดือน",K34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K51:K55">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="รายเดือน">
-      <formula>NOT(ISERROR(SEARCH("รายเดือน",K51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J21:J33 J37:J49 J2:J19 J56:J63">
-    <cfRule type="containsText" dxfId="1" priority="10" operator="containsText" text="เงินสด">
+  <conditionalFormatting sqref="J2:J95">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="เงินสด">
       <formula>NOT(ISERROR(SEARCH("เงินสด",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K18 K21:K33 K37:K49 K57:K64">
-    <cfRule type="containsText" dxfId="0" priority="11" operator="containsText" text="รายเดือน">
+  <conditionalFormatting sqref="K2:K95">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="รายเดือน">
       <formula>NOT(ISERROR(SEARCH("รายเดือน",K2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>